<commit_message>
finalized new tool workflow, started on trip to place conversion
</commit_message>
<xml_diff>
--- a/documents/SPA_input_tables.xlsx
+++ b/documents/SPA_input_tables.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25809"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david.hensle\Documents\reports\Translink\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitclones\Dubai_survey_processing\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B563674-B1AD-46A8-9F6A-A156E9CCFD11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186133E4-CD4D-449C-8277-83B180A0015B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="3" activeTab="3" xr2:uid="{F3EA6906-BC25-417E-92D1-3F0826AA48EE}"/>
+    <workbookView xWindow="4185" yWindow="285" windowWidth="23835" windowHeight="14700" activeTab="2" xr2:uid="{F3EA6906-BC25-417E-92D1-3F0826AA48EE}"/>
   </bookViews>
   <sheets>
     <sheet name="households" sheetId="1" r:id="rId1"/>
     <sheet name="persons" sheetId="2" r:id="rId2"/>
     <sheet name="trips" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="place" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="132">
   <si>
     <t>Field Name</t>
   </si>
@@ -430,12 +431,73 @@
   <si>
     <t>Social/Visit</t>
   </si>
+  <si>
+    <t>DAYNO</t>
+  </si>
+  <si>
+    <t>YCORD</t>
+  </si>
+  <si>
+    <t>XCORD</t>
+  </si>
+  <si>
+    <t>WXCORD</t>
+  </si>
+  <si>
+    <t>WYCORD</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Day Number </t>
+  </si>
+  <si>
+    <t>Work Y coordinate</t>
+  </si>
+  <si>
+    <t>Work X Coordinate</t>
+  </si>
+  <si>
+    <t>Place X Coordinate</t>
+  </si>
+  <si>
+    <t>Place Y Coordinate</t>
+  </si>
+  <si>
+    <t>AGE_CAT</t>
+  </si>
+  <si>
+    <t>Age category</t>
+  </si>
+  <si>
+    <t>1: &lt;5
+2: 5-15
+3: 16-17
+4: 18-24
+5: 25-34
+6: 35-44
+7: 45-49
+8: 50-54
+9: 55-59
+10: 60-64
+11: 65-74
+12: 75-79
+13: 80-84
+14: &gt;85</t>
+  </si>
+  <si>
+    <t>DISTANCE</t>
+  </si>
+  <si>
+    <t>Trip distance in km</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,7 +526,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -482,6 +544,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -802,10 +865,10 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
@@ -813,7 +876,7 @@
     <col min="4" max="4" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -827,7 +890,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -841,7 +904,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -852,7 +915,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -863,7 +926,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -874,7 +937,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -885,7 +948,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -903,20 +966,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C287D932-C797-499C-8452-8AF9C419046E}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -930,7 +993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -944,7 +1007,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -958,7 +1021,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -972,7 +1035,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -986,7 +1049,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.9">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -998,7 +1061,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="43.15">
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1012,7 +1075,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="172.9">
+    <row r="8" spans="1:4" ht="195" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -1026,7 +1089,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="57.6">
+    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -1040,7 +1103,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
@@ -1052,33 +1115,50 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="28.9">
+    <row r="11" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="57.6">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>49</v>
       </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1087,20 +1167,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E27602A-329C-4795-A79E-F4DC0F2A8061}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.28515625" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1114,7 +1194,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1128,7 +1208,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1142,7 +1222,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>50</v>
       </c>
@@ -1156,7 +1236,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.9">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -1167,7 +1247,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>55</v>
       </c>
@@ -1178,7 +1258,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="201.6">
+    <row r="7" spans="1:4" ht="210" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1192,7 +1272,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="158.44999999999999">
+    <row r="8" spans="1:4" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>60</v>
       </c>
@@ -1206,189 +1286,201 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.9">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28.9">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28.9">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="28.9">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.9">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="3" t="s">
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.9">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B18" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="43.15">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28.9">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="43.15">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="3" t="s">
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.9">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.9">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="3" t="s">
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1398,14 +1490,191 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B44E6E7-8C75-451F-88FB-1DFB409AF133}">
+  <dimension ref="A1:D81"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="2"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+    </row>
+    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="2"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
+    </row>
+    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="2"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="2"/>
+      <c r="C79" s="3"/>
+      <c r="D79" s="3"/>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B80" s="2"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B81" s="2"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DDFCF6-68F7-438A-A8C4-07D67CA10D4B}">
   <dimension ref="B3:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
@@ -1415,24 +1684,24 @@
     <col min="6" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12">
-      <c r="B3" s="7" t="s">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-    </row>
-    <row r="4" spans="2:12">
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>100</v>
       </c>
@@ -1467,7 +1736,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>110</v>
       </c>
@@ -1502,7 +1771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>4</v>
       </c>
@@ -1537,7 +1806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <v>44322</v>
       </c>
@@ -1572,7 +1841,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
@@ -1607,7 +1876,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
created place from trip conversion
</commit_message>
<xml_diff>
--- a/documents/SPA_input_tables.xlsx
+++ b/documents/SPA_input_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\gitclones\Dubai_survey_processing\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186133E4-CD4D-449C-8277-83B180A0015B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1582132-629E-4DB0-9661-308470217BD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="285" windowWidth="23835" windowHeight="14700" activeTab="2" xr2:uid="{F3EA6906-BC25-417E-92D1-3F0826AA48EE}"/>
+    <workbookView xWindow="3733" yWindow="220" windowWidth="21807" windowHeight="12280" activeTab="3" xr2:uid="{F3EA6906-BC25-417E-92D1-3F0826AA48EE}"/>
   </bookViews>
   <sheets>
     <sheet name="households" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="135">
   <si>
     <t>Field Name</t>
   </si>
@@ -491,6 +491,15 @@
   </si>
   <si>
     <t>Trip distance in km</t>
+  </si>
+  <si>
+    <t>PNAME</t>
+  </si>
+  <si>
+    <t>STR</t>
+  </si>
+  <si>
+    <t>Plane Name</t>
   </si>
 </sst>
 </file>
@@ -868,15 +877,15 @@
       <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.703125" customWidth="1"/>
     <col min="3" max="3" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.29296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -890,7 +899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -904,7 +913,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -915,7 +924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -926,7 +935,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -937,7 +946,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -948,7 +957,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -968,18 +977,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C287D932-C797-499C-8452-8AF9C419046E}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="25.29296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.29296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -993,7 +1002,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1007,7 +1016,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1021,7 +1030,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
@@ -1035,7 +1044,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1049,7 +1058,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>31</v>
       </c>
@@ -1061,7 +1070,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="43" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>33</v>
       </c>
@@ -1075,7 +1084,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="195" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="172" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -1089,7 +1098,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
         <v>39</v>
       </c>
@@ -1103,7 +1112,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
@@ -1115,7 +1124,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="200.7" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
         <v>127</v>
       </c>
@@ -1129,7 +1138,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="s">
         <v>44</v>
       </c>
@@ -1143,7 +1152,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="57.35" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
@@ -1157,7 +1166,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.5">
       <c r="F17" s="7"/>
     </row>
   </sheetData>
@@ -1169,18 +1178,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E27602A-329C-4795-A79E-F4DC0F2A8061}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.29296875" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1194,7 +1203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1208,7 +1217,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1222,7 +1231,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" s="2" t="s">
         <v>50</v>
       </c>
@@ -1236,7 +1245,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -1247,7 +1256,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" s="2" t="s">
         <v>55</v>
       </c>
@@ -1258,7 +1267,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="210" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="200.7" x14ac:dyDescent="0.5">
       <c r="A7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1272,7 +1281,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="157.69999999999999" x14ac:dyDescent="0.5">
       <c r="A8" s="2" t="s">
         <v>60</v>
       </c>
@@ -1286,7 +1295,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" s="2" t="s">
         <v>130</v>
       </c>
@@ -1298,7 +1307,7 @@
       </c>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" s="2" t="s">
         <v>63</v>
       </c>
@@ -1312,7 +1321,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -1326,7 +1335,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A12" s="2" t="s">
         <v>69</v>
       </c>
@@ -1340,7 +1349,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A13" s="2" t="s">
         <v>71</v>
       </c>
@@ -1354,7 +1363,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A14" s="2" t="s">
         <v>73</v>
       </c>
@@ -1368,7 +1377,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A15" s="2" t="s">
         <v>76</v>
       </c>
@@ -1382,7 +1391,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A16" s="2" t="s">
         <v>79</v>
       </c>
@@ -1393,7 +1402,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A17" s="2" t="s">
         <v>81</v>
       </c>
@@ -1407,7 +1416,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A18" s="2" t="s">
         <v>84</v>
       </c>
@@ -1418,7 +1427,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A19" s="2" t="s">
         <v>86</v>
       </c>
@@ -1429,7 +1438,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="43" x14ac:dyDescent="0.5">
       <c r="A20" s="2" t="s">
         <v>88</v>
       </c>
@@ -1440,7 +1449,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A21" s="2" t="s">
         <v>90</v>
       </c>
@@ -1451,7 +1460,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A22" s="2" t="s">
         <v>92</v>
       </c>
@@ -1462,7 +1471,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A23" s="2" t="s">
         <v>94</v>
       </c>
@@ -1473,7 +1482,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
       <c r="A24" s="2" t="s">
         <v>96</v>
       </c>
@@ -1491,21 +1500,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B44E6E7-8C75-451F-88FB-1DFB409AF133}">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.87890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.29296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.87890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>121</v>
       </c>
@@ -1519,7 +1528,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1533,7 +1542,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1547,7 +1556,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -1561,7 +1570,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -1575,94 +1584,195 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="157.69999999999999" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
         <v>117</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
         <v>118</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
         <v>119</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
         <v>120</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C13" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="210" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="14" spans="1:4" ht="200.7" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
         <v>57</v>
       </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B76" s="2"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B77" s="2"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B78" s="2"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="3"/>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B79" s="2"/>
-      <c r="C79" s="3"/>
-      <c r="D79" s="3"/>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A18" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="80" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B80" s="2"/>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.5">
       <c r="B81" s="2"/>
       <c r="C81" s="3"/>
-      <c r="D81" s="1"/>
+      <c r="D81" s="3"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B82" s="2"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B83" s="2"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B84" s="2"/>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.5">
+      <c r="B85" s="2"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1674,17 +1784,17 @@
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.29296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.29296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.29296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="7.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.5">
       <c r="B3" s="8" t="s">
         <v>98</v>
       </c>
@@ -1701,7 +1811,7 @@
       <c r="K3" s="8"/>
       <c r="L3" s="8"/>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.5">
       <c r="B4" t="s">
         <v>100</v>
       </c>
@@ -1736,7 +1846,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.5">
       <c r="B5" t="s">
         <v>110</v>
       </c>
@@ -1771,7 +1881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.5">
       <c r="B6">
         <v>4</v>
       </c>
@@ -1806,7 +1916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.5">
       <c r="B7" s="6">
         <v>44322</v>
       </c>
@@ -1841,7 +1951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.5">
       <c r="B8">
         <v>7</v>
       </c>
@@ -1876,7 +1986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.5">
       <c r="B9">
         <v>8</v>
       </c>

</xml_diff>